<commit_message>
added downward euler and pressure integration
</commit_message>
<xml_diff>
--- a/Planetary datasheet.xlsx
+++ b/Planetary datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bartroot/TUDelft/Education/3. Course/Physics of Planetary Interiors/Lectures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ward/Documents/GitHub/Ward-github/PPI/PPIAssignment1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC3FE6D-8B9E-F742-ADD1-D82934DED594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679216FD-A005-2749-ABB0-FA3874C1906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{1146C626-9A0D-214B-A53F-A7E8915953E9}"/>
+    <workbookView xWindow="840" yWindow="620" windowWidth="27960" windowHeight="16220" xr2:uid="{1146C626-9A0D-214B-A53F-A7E8915953E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +358,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,15 +616,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D6AC61-59A9-B544-8F61-6E655A81509B}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="16.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.33203125" style="1" customWidth="1"/>

</xml_diff>